<commit_message>
initial push for IAU 2015 report (minor updates to 2009 files)
</commit_message>
<xml_diff>
--- a/OGC_IAU2000_WKT_v2/Source_Python/naifcodes_radii_m_wAsteroids_IAU2009.xlsx
+++ b/OGC_IAU2000_WKT_v2/Source_Python/naifcodes_radii_m_wAsteroids_IAU2009.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trent\Downloads\GDAL_scripts-master\OGC_IAU2000_WKT_v2\Source_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thare\Documents\GIT\GDAL_scripts\OGC_IAU2000_WKT_v2\Source_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -459,9 +459,6 @@
     <t>Methone</t>
   </si>
   <si>
-    <t>IAU2000_Axisb</t>
-  </si>
-  <si>
     <t>Daphnis</t>
   </si>
   <si>
@@ -568,6 +565,9 @@
   </si>
   <si>
     <t>Wild 2</t>
+  </si>
+  <si>
+    <t>IAU2009_Axisb</t>
   </si>
 </sst>
 </file>
@@ -1052,10 +1052,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1437,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,7 +1466,7 @@
         <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>143</v>
@@ -2596,7 +2597,7 @@
         <v>549</v>
       </c>
       <c r="B58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C58" s="2">
         <v>-1</v>
@@ -2616,7 +2617,7 @@
         <v>550</v>
       </c>
       <c r="B59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C59" s="2">
         <v>-1</v>
@@ -3336,7 +3337,7 @@
         <v>635</v>
       </c>
       <c r="B95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C95" s="1">
         <v>3800</v>
@@ -3348,7 +3349,7 @@
         <v>4100</v>
       </c>
       <c r="F95" s="1">
-        <v>9400</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3356,7 +3357,7 @@
         <v>636</v>
       </c>
       <c r="B96" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C96" s="2">
         <v>-1</v>
@@ -3376,7 +3377,7 @@
         <v>637</v>
       </c>
       <c r="B97" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C97" s="2">
         <v>-1</v>
@@ -3396,7 +3397,7 @@
         <v>638</v>
       </c>
       <c r="B98" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C98" s="2">
         <v>-1</v>
@@ -3416,7 +3417,7 @@
         <v>639</v>
       </c>
       <c r="B99" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C99" s="2">
         <v>-1</v>
@@ -3436,7 +3437,7 @@
         <v>640</v>
       </c>
       <c r="B100" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C100" s="2">
         <v>-1</v>
@@ -3456,7 +3457,7 @@
         <v>641</v>
       </c>
       <c r="B101" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C101" s="2">
         <v>-1</v>
@@ -3476,7 +3477,7 @@
         <v>642</v>
       </c>
       <c r="B102" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C102" s="2">
         <v>-1</v>
@@ -3496,7 +3497,7 @@
         <v>643</v>
       </c>
       <c r="B103" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C103" s="2">
         <v>-1</v>
@@ -3516,7 +3517,7 @@
         <v>644</v>
       </c>
       <c r="B104" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C104" s="2">
         <v>-1</v>
@@ -3536,7 +3537,7 @@
         <v>645</v>
       </c>
       <c r="B105" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C105" s="2">
         <v>-1</v>
@@ -3556,7 +3557,7 @@
         <v>646</v>
       </c>
       <c r="B106" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C106" s="2">
         <v>-1</v>
@@ -3576,7 +3577,7 @@
         <v>647</v>
       </c>
       <c r="B107" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C107" s="2">
         <v>-1</v>
@@ -3596,7 +3597,7 @@
         <v>648</v>
       </c>
       <c r="B108" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C108" s="2">
         <v>-1</v>
@@ -3616,7 +3617,7 @@
         <v>649</v>
       </c>
       <c r="B109" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C109" s="1">
         <v>1000</v>
@@ -3636,7 +3637,7 @@
         <v>650</v>
       </c>
       <c r="B110" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C110" s="2">
         <v>-1</v>
@@ -3656,7 +3657,7 @@
         <v>651</v>
       </c>
       <c r="B111" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C111" s="2">
         <v>-1</v>
@@ -3676,7 +3677,7 @@
         <v>652</v>
       </c>
       <c r="B112" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C112" s="2">
         <v>-1</v>
@@ -3696,7 +3697,7 @@
         <v>653</v>
       </c>
       <c r="B113" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C113" s="2">
         <v>-1</v>
@@ -4156,7 +4157,7 @@
         <v>722</v>
       </c>
       <c r="B136" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C136" s="2">
         <v>-1</v>
@@ -4176,7 +4177,7 @@
         <v>723</v>
       </c>
       <c r="B137" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C137" s="2">
         <v>-1</v>
@@ -4196,7 +4197,7 @@
         <v>724</v>
       </c>
       <c r="B138" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C138" s="2">
         <v>-1</v>
@@ -4216,7 +4217,7 @@
         <v>725</v>
       </c>
       <c r="B139" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C139" s="2">
         <v>-1</v>
@@ -4236,7 +4237,7 @@
         <v>726</v>
       </c>
       <c r="B140" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C140" s="2">
         <v>-1</v>
@@ -4256,7 +4257,7 @@
         <v>727</v>
       </c>
       <c r="B141" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C141" s="2">
         <v>-1</v>
@@ -4456,7 +4457,7 @@
         <v>809</v>
       </c>
       <c r="B151" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C151" s="2">
         <v>-1</v>
@@ -4476,7 +4477,7 @@
         <v>810</v>
       </c>
       <c r="B152" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C152" s="2">
         <v>-1</v>
@@ -4496,7 +4497,7 @@
         <v>811</v>
       </c>
       <c r="B153" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C153" s="2">
         <v>-1</v>
@@ -4516,7 +4517,7 @@
         <v>812</v>
       </c>
       <c r="B154" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C154" s="2">
         <v>-1</v>
@@ -4536,7 +4537,7 @@
         <v>813</v>
       </c>
       <c r="B155" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C155" s="2">
         <v>-1</v>
@@ -4596,7 +4597,7 @@
         <v>1000005</v>
       </c>
       <c r="B158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C158" s="1">
         <v>4220</v>
@@ -4616,9 +4617,9 @@
         <v>1000036</v>
       </c>
       <c r="B159" t="s">
-        <v>180</v>
-      </c>
-      <c r="C159" s="1">
+        <v>179</v>
+      </c>
+      <c r="C159" s="3">
         <v>-1</v>
       </c>
       <c r="D159" s="1">
@@ -4636,7 +4637,7 @@
         <v>1000093</v>
       </c>
       <c r="B160" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C160" s="1">
         <v>3000</v>
@@ -4656,7 +4657,7 @@
         <v>1000107</v>
       </c>
       <c r="B161" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C161" s="1">
         <v>1975</v>

</xml_diff>